<commit_message>
pre covid and preg on new db
</commit_message>
<xml_diff>
--- a/data/V15_COVID19/covid_phenotype/COVID_ICD.xlsx
+++ b/data/V15_COVID19/covid_phenotype/COVID_ICD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zangc\PycharmProjects\pasc\data\V15_COVID19\covid_phenotype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zangc\PycharmProjects\pasc_phenotype\data\V15_COVID19\covid_phenotype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BEA5F4-8670-4376-AEC8-74AAEBDD8969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BA2A5E-CC46-499E-AAB3-05C6C55BF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -771,18 +771,18 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
+    <col min="2" max="2" width="69.42578125" customWidth="1"/>
     <col min="3" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>91</v>
       </c>
@@ -828,7 +828,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>30</v>
       </c>
@@ -852,7 +852,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
@@ -876,7 +876,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>19</v>
       </c>
@@ -900,7 +900,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -922,7 +922,7 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
@@ -946,7 +946,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1040,15 +1040,15 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="55.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>40</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>45</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>50</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>55</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>8.3624708624708624E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>60</v>
       </c>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>62</v>
       </c>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>64</v>
       </c>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>66</v>
       </c>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>70</v>
       </c>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>72</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>74</v>
       </c>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>76</v>
       </c>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>78</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>80</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>82</v>
       </c>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>84</v>
       </c>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>86</v>
       </c>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>88</v>
       </c>

</xml_diff>